<commit_message>
updated historical cp discharge
</commit_message>
<xml_diff>
--- a/Control point historical discharge 2005.xlsx
+++ b/Control point historical discharge 2005.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Albany" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Foster" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6273,7 +6274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9228,7 +9229,7 @@
   <dimension ref="A1:B367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15135,7 +15136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>